<commit_message>
Add username/password validation tests
Add tests related to SQL Injection. No Valid SQL Statement
should be submittable as a username or password (mainly
because spaces are not allowed in either). Additionaly only
the encrypted version of the password is stored.

Also add missing newline at the end of several files.

Closes #14
</commit_message>
<xml_diff>
--- a/machinarium/src/test/resources/validators/TestData.xlsx
+++ b/machinarium/src/test/resources/validators/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zukad\OneDrive\Desktop\OOP_Project\machinarium\src\test\resources\validators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EF77E1F6-16D0-4078-B617-592D0E50BA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D47A2151-297B-4CDA-BB00-9B2AD15D4B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UsernameValidatorTestData" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="65" uniqueCount="48">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="81" uniqueCount="57">
   <si>
     <t>Expected Result</t>
   </si>
@@ -174,6 +174,34 @@
   <si>
     <t>adb1
 AAA</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Non-Empty Marker</t>
+  </si>
+  <si>
+    <t>DROP TABLE Users;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT </t>
+  </si>
+  <si>
+    <t>SELECT * FROM Users;</t>
+  </si>
+  <si>
+    <t>DROP DATABASE Machinarium;</t>
+  </si>
+  <si>
+    <t>UPDATE Users SET password="c748db15ab47dfba758ceedf0655043585372cf5cc64388cb9710c3e93959544";</t>
+  </si>
+  <si>
+    <t>INSERT INTO Users(username, password)
+VALUES ("someguyiwannahack", "Easy_Password123");</t>
+  </si>
+  <si>
+    <t>DELETE FROM Users;</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1108,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1117,7 +1145,7 @@
         <v>INVALID</v>
       </c>
       <c r="D6" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$5&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
         <v>Contains at least 4 characters.</v>
       </c>
     </row>
@@ -1134,7 +1162,7 @@
         <v>INVALID</v>
       </c>
       <c r="D7" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$5&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
         <v>Contains at least 4 characters.</v>
       </c>
     </row>
@@ -1168,6 +1196,140 @@
       </c>
       <c r="D9" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
       </c>
     </row>
   </sheetData>
@@ -1178,16 +1340,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="97" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
     <col min="4" max="4" width="64.7109375" style="1" customWidth="1"/>
   </cols>
@@ -1233,7 +1395,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A23" si="0">A3+1</f>
+        <f t="shared" ref="A4:A32" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1462,7 +1624,7 @@
         <v>INVALID</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1479,7 +1641,7 @@
         <v>INVALID</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1496,7 +1658,7 @@
         <v>INVALID</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1546,6 +1708,139 @@
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f>'Configurable Data'!$B$4</f>
+        <v>*</v>
       </c>
     </row>
   </sheetData>
@@ -1557,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,19 +1888,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>42</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add test cases for space-less SQL injections
</commit_message>
<xml_diff>
--- a/machinarium/src/test/resources/validators/TestData.xlsx
+++ b/machinarium/src/test/resources/validators/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zukad\OneDrive\Desktop\OOP_Project\machinarium\src\test\resources\validators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D47A2151-297B-4CDA-BB00-9B2AD15D4B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FD9735AC-4ABD-4DB3-ADCE-52AFD65209DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="81" uniqueCount="57">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="116" uniqueCount="62">
   <si>
     <t>Expected Result</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>DELETE FROM Users;</t>
+  </si>
+  <si>
+    <t>SELECT/*avoid-spaces*/password/**/FROM/**/Members</t>
+  </si>
+  <si>
+    <t>Contains at least 4 characters.</t>
+  </si>
+  <si>
+    <t>select'asdf'as[asdf]into[#MyTable]</t>
+  </si>
+  <si>
+    <t>DELETE/**/FROM/**/Users</t>
+  </si>
+  <si>
+    <t>exec[sp_executesql]N'select''asdf''as[asdf]into[#MyTable]'</t>
   </si>
 </sst>
 </file>
@@ -691,11 +706,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1053,16 +1071,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="93.85546875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" customWidth="1"/>
   </cols>
@@ -1071,13 +1089,13 @@
       <c r="A1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1088,95 +1106,80 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f>'Configurable Data'!$B$2</f>
-        <v>VALID</v>
+      <c r="C2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f>'Configurable Data'!$B$2</f>
-        <v>VALID</v>
+      <c r="C3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f>'Configurable Data'!$B$2</f>
-        <v>VALID</v>
+      <c r="C4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f>'Configurable Data'!$B$2</f>
-        <v>VALID</v>
+      <c r="C5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D6" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
-        <v>Contains at least 4 characters.</v>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D7" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$6&amp;" characters."</f>
-        <v>Contains at least 4 characters.</v>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -1184,15 +1187,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
+      <c r="C9" t="s">
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -1200,136 +1201,153 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f>'Configurable Data'!$B$3</f>
-        <v>INVALID</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f>'Configurable Data'!$B$4</f>
-        <v>*</v>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1395,7 +1413,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A32" si="0">A3+1</f>
+        <f t="shared" ref="A4:A31" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">

</xml_diff>

<commit_message>
Add max length validation for username/password
</commit_message>
<xml_diff>
--- a/machinarium/src/test/resources/validators/TestData.xlsx
+++ b/machinarium/src/test/resources/validators/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zukad\OneDrive\Desktop\OOP_Project\machinarium\src\test\resources\validators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FD9735AC-4ABD-4DB3-ADCE-52AFD65209DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{33DB7E32-5F0C-4919-A3DD-684D0B121742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UsernameValidatorTestData" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="116" uniqueCount="62">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="127" uniqueCount="72">
   <si>
     <t>Expected Result</t>
   </si>
@@ -217,6 +217,36 @@
   </si>
   <si>
     <t>exec[sp_executesql]N'select''asdf''as[asdf]into[#MyTable]'</t>
+  </si>
+  <si>
+    <t>Maximum Username Length</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Maximum Password Length</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb vkwda___WD?A?WD?DdawdD?W????a</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb vkwda___WD?A?WD?DdawdD?W????ab</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb vkwda___WD?A?WD?DdawdD?W????abc</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb_vkwda___WD_A_WD_DdawdD_W____ab</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb_vkwda___WD_A_WD_DdawdD_W____a</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad123131231333333333341241jkfhawdb_vkwda___WD_A_WD_DdawdD_W____abc</t>
+  </si>
+  <si>
+    <t>madeup_passADWAWDawdawdawdwadwadwadad1</t>
   </si>
 </sst>
 </file>
@@ -706,7 +736,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -716,6 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1071,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,6 +1381,51 @@
         <v>23</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" ref="A21:A23" si="0">A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>'Configurable Data'!$B$2</f>
+        <v>VALID</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>'Configurable Data'!$B$2</f>
+        <v>VALID</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f>"Doesn't contain more than "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
+        <v>Doesn't contain more than 100 characters.</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1358,10 +1434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1489,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A31" si="0">A3+1</f>
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1642,7 +1718,7 @@
         <v>INVALID</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$8&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1659,7 +1735,7 @@
         <v>INVALID</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$8&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1676,7 +1752,7 @@
         <v>INVALID</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f>"Contains at least "&amp;'Configurable Data'!$B$7&amp;" characters."</f>
+        <f>"Contains at least "&amp;'Configurable Data'!$B$8&amp;" characters."</f>
         <v>Contains at least 8 characters.</v>
       </c>
     </row>
@@ -1859,6 +1935,62 @@
       <c r="D31" s="1" t="str">
         <f>'Configurable Data'!$B$4</f>
         <v>*</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="1" t="str">
+        <f>'Configurable Data'!$B$2</f>
+        <v>VALID</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f>'Configurable Data'!$B$2</f>
+        <v>VALID</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f>'Configurable Data'!$B$2</f>
+        <v>VALID</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f>'Configurable Data'!$B$3</f>
+        <v>INVALID</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <f>"Doesn't contain more than "&amp;'Configurable Data'!$B$9&amp;" characters."</f>
+        <v>Doesn't contain more than 100 characters.</v>
       </c>
     </row>
   </sheetData>
@@ -1870,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,10 +2056,26 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>